<commit_message>
Mono city files prep (19-21)
Need to check
</commit_message>
<xml_diff>
--- a/migforecasting/cities19-21/d2.xlsx
+++ b/migforecasting/cities19-21/d2.xlsx
@@ -1,10 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Albert\.spyder-py3\ITMO-2\migforecasting\cities19-21\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="480" yWindow="75" windowWidth="27795" windowHeight="12345"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12885"/>
   </bookViews>
   <sheets>
     <sheet name="Лист1" sheetId="1" r:id="rId1"/>
@@ -19,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="143" uniqueCount="121">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="144" uniqueCount="122">
   <si>
     <t>обеспечение электрической энергией, газом и паром;  кондиционирование воздуха</t>
   </si>
@@ -1008,16 +1013,19 @@
       </rPr>
       <t>1)</t>
     </r>
+  </si>
+  <si>
+    <t>Брянск</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="#,##0.0"/>
   </numFmts>
-  <fonts count="9" x14ac:knownFonts="1">
+  <fonts count="9">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1286,6 +1294,60 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1" indent="5"/>
+    </xf>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1" indent="5"/>
+    </xf>
+    <xf numFmtId="164" fontId="8" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1" indent="5"/>
+    </xf>
+    <xf numFmtId="164" fontId="8" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1" indent="5"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1" indent="5"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1" indent="5"/>
+    </xf>
+    <xf numFmtId="164" fontId="8" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1" indent="5"/>
+    </xf>
+    <xf numFmtId="164" fontId="8" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1" indent="5"/>
+    </xf>
+    <xf numFmtId="3" fontId="1" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1" indent="5"/>
+    </xf>
+    <xf numFmtId="3" fontId="1" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1" indent="5"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -1294,60 +1356,6 @@
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="1" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1" indent="5"/>
-    </xf>
-    <xf numFmtId="164" fontId="1" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1" indent="5"/>
-    </xf>
-    <xf numFmtId="164" fontId="8" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1" indent="5"/>
-    </xf>
-    <xf numFmtId="164" fontId="8" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1" indent="5"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1" indent="5"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1" indent="5"/>
-    </xf>
-    <xf numFmtId="164" fontId="8" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1" indent="5"/>
-    </xf>
-    <xf numFmtId="164" fontId="8" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1" indent="5"/>
-    </xf>
-    <xf numFmtId="3" fontId="1" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1" indent="5"/>
-    </xf>
-    <xf numFmtId="3" fontId="1" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1" indent="5"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1358,6 +1366,9 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -1406,7 +1417,7 @@
     </a:clrScheme>
     <a:fontScheme name="Стандартная">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1441,7 +1452,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1653,25 +1664,27 @@
   <dimension ref="A1:D86"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection sqref="A1:D1"/>
+      <selection activeCell="J9" sqref="J9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="57.140625" customWidth="1"/>
     <col min="2" max="4" width="17.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A1" s="16" t="s">
+    <row r="1" spans="1:4">
+      <c r="A1" s="27" t="s">
         <v>120</v>
       </c>
-      <c r="B1" s="16"/>
-      <c r="C1" s="16"/>
-      <c r="D1" s="16"/>
-    </row>
-    <row r="2" spans="1:4" ht="12.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="9"/>
+      <c r="B1" s="27"/>
+      <c r="C1" s="27"/>
+      <c r="D1" s="27"/>
+    </row>
+    <row r="2" spans="1:4" ht="12.95" customHeight="1">
+      <c r="A2" s="9" t="s">
+        <v>121</v>
+      </c>
       <c r="B2" s="1">
         <v>2019</v>
       </c>
@@ -1682,327 +1695,327 @@
         <v>2021</v>
       </c>
     </row>
-    <row r="3" spans="1:4" ht="12.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="10" t="s">
+    <row r="3" spans="1:4" ht="12.95" customHeight="1">
+      <c r="A3" s="28" t="s">
         <v>1</v>
       </c>
-      <c r="B3" s="11"/>
-      <c r="C3" s="11"/>
-      <c r="D3" s="12"/>
-    </row>
-    <row r="4" spans="1:4" ht="12.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B3" s="29"/>
+      <c r="C3" s="29"/>
+      <c r="D3" s="30"/>
+    </row>
+    <row r="4" spans="1:4" ht="12.95" customHeight="1">
       <c r="A4" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="B4" s="17">
+      <c r="B4" s="10">
         <v>420.4</v>
       </c>
-      <c r="C4" s="17">
+      <c r="C4" s="10">
         <v>417.1</v>
       </c>
-      <c r="D4" s="18">
+      <c r="D4" s="11">
         <v>413.4</v>
       </c>
     </row>
-    <row r="5" spans="1:4" ht="12.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:4" ht="12.95" customHeight="1">
       <c r="A5" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="B5" s="17"/>
-      <c r="C5" s="17"/>
-      <c r="D5" s="18"/>
-    </row>
-    <row r="6" spans="1:4" ht="12.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B5" s="10"/>
+      <c r="C5" s="10"/>
+      <c r="D5" s="11"/>
+    </row>
+    <row r="6" spans="1:4" ht="12.95" customHeight="1">
       <c r="A6" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="B6" s="19">
+      <c r="B6" s="12">
         <v>69.099999999999994</v>
       </c>
-      <c r="C6" s="19">
+      <c r="C6" s="12">
         <v>69.2</v>
       </c>
-      <c r="D6" s="20">
+      <c r="D6" s="13">
         <v>69</v>
       </c>
     </row>
-    <row r="7" spans="1:4" ht="12.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:4" ht="12.95" customHeight="1">
       <c r="A7" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="B7" s="19">
+      <c r="B7" s="12">
         <v>27.1</v>
       </c>
-      <c r="C7" s="19">
+      <c r="C7" s="12">
         <v>26.9</v>
       </c>
-      <c r="D7" s="20">
+      <c r="D7" s="13">
         <v>26.5</v>
       </c>
     </row>
-    <row r="8" spans="1:4" ht="12.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:4" ht="12.95" customHeight="1">
       <c r="A8" s="6" t="s">
         <v>38</v>
       </c>
-      <c r="B8" s="19">
+      <c r="B8" s="12">
         <v>233.9</v>
       </c>
-      <c r="C8" s="19">
+      <c r="C8" s="12">
         <v>229.4</v>
       </c>
-      <c r="D8" s="20">
+      <c r="D8" s="13">
         <v>232</v>
       </c>
     </row>
-    <row r="9" spans="1:4" ht="12.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:4" ht="12.95" customHeight="1">
       <c r="A9" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="B9" s="19">
+      <c r="B9" s="12">
         <v>117.4</v>
       </c>
-      <c r="C9" s="19">
+      <c r="C9" s="12">
         <v>118.5</v>
       </c>
-      <c r="D9" s="20">
+      <c r="D9" s="13">
         <v>112.4</v>
       </c>
     </row>
-    <row r="10" spans="1:4" ht="12.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:4" ht="12.95" customHeight="1">
       <c r="A10" s="3" t="s">
         <v>39</v>
       </c>
-      <c r="B10" s="17">
+      <c r="B10" s="10">
         <v>9.9</v>
       </c>
-      <c r="C10" s="17">
+      <c r="C10" s="10">
         <v>9</v>
       </c>
-      <c r="D10" s="18">
+      <c r="D10" s="11">
         <v>8.6999999999999993</v>
       </c>
     </row>
-    <row r="11" spans="1:4" ht="12.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:4" ht="12.95" customHeight="1">
       <c r="A11" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="B11" s="17">
+      <c r="B11" s="10">
         <v>13.4</v>
       </c>
-      <c r="C11" s="17">
+      <c r="C11" s="10">
         <v>16.2</v>
       </c>
-      <c r="D11" s="18">
+      <c r="D11" s="11">
         <v>20.2</v>
       </c>
     </row>
-    <row r="12" spans="1:4" ht="12.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:4" ht="12.95" customHeight="1">
       <c r="A12" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="B12" s="17">
+      <c r="B12" s="10">
         <v>-3.5</v>
       </c>
-      <c r="C12" s="17">
+      <c r="C12" s="10">
         <v>-7.2</v>
       </c>
-      <c r="D12" s="18">
+      <c r="D12" s="11">
         <v>-11.5</v>
       </c>
     </row>
-    <row r="13" spans="1:4" ht="12.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:4" ht="12.95" customHeight="1">
       <c r="A13" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="B13" s="17">
+      <c r="B13" s="10">
         <v>-877</v>
       </c>
-      <c r="C13" s="17">
+      <c r="C13" s="10">
         <v>54</v>
       </c>
-      <c r="D13" s="18" t="s">
+      <c r="D13" s="11" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="14" spans="1:4" ht="12.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="13" t="s">
+    <row r="14" spans="1:4" ht="12.95" customHeight="1">
+      <c r="A14" s="23" t="s">
         <v>10</v>
       </c>
-      <c r="B14" s="14"/>
-      <c r="C14" s="14"/>
-      <c r="D14" s="15"/>
-    </row>
-    <row r="15" spans="1:4" ht="12.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B14" s="24"/>
+      <c r="C14" s="24"/>
+      <c r="D14" s="25"/>
+    </row>
+    <row r="15" spans="1:4" ht="12.95" customHeight="1">
       <c r="A15" s="3" t="s">
         <v>41</v>
       </c>
-      <c r="B15" s="19">
+      <c r="B15" s="12">
         <v>117.1</v>
       </c>
-      <c r="C15" s="19">
+      <c r="C15" s="12">
         <v>115.2</v>
       </c>
-      <c r="D15" s="20">
+      <c r="D15" s="13">
         <v>114.3</v>
       </c>
     </row>
-    <row r="16" spans="1:4" ht="23.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:4" ht="23.1" customHeight="1">
       <c r="A16" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="B16" s="21" t="s">
+      <c r="B16" s="14" t="s">
         <v>42</v>
       </c>
-      <c r="C16" s="21" t="s">
+      <c r="C16" s="14" t="s">
         <v>43</v>
       </c>
-      <c r="D16" s="22" t="s">
+      <c r="D16" s="15" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="17" spans="1:4" ht="12.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:4" ht="12.95" customHeight="1">
       <c r="A17" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="B17" s="21" t="s">
+      <c r="B17" s="14" t="s">
         <v>45</v>
       </c>
-      <c r="C17" s="21" t="s">
+      <c r="C17" s="14" t="s">
         <v>46</v>
       </c>
-      <c r="D17" s="22" t="s">
+      <c r="D17" s="15" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="18" spans="1:4" ht="12.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="13" t="s">
+    <row r="18" spans="1:4" ht="12.95" customHeight="1">
+      <c r="A18" s="23" t="s">
         <v>13</v>
       </c>
-      <c r="B18" s="14"/>
-      <c r="C18" s="14"/>
-      <c r="D18" s="15"/>
-    </row>
-    <row r="19" spans="1:4" ht="23.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B18" s="24"/>
+      <c r="C18" s="24"/>
+      <c r="D18" s="25"/>
+    </row>
+    <row r="19" spans="1:4" ht="23.1" customHeight="1">
       <c r="A19" s="3" t="s">
         <v>48</v>
       </c>
-      <c r="B19" s="19" t="s">
+      <c r="B19" s="12" t="s">
         <v>49</v>
       </c>
-      <c r="C19" s="19">
+      <c r="C19" s="12">
         <v>38825.599999999999</v>
       </c>
-      <c r="D19" s="20">
+      <c r="D19" s="13">
         <v>42430.2</v>
       </c>
     </row>
-    <row r="20" spans="1:4" ht="12.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:4" ht="12.95" customHeight="1">
       <c r="A20" s="3" t="s">
         <v>50</v>
       </c>
-      <c r="B20" s="19" t="s">
+      <c r="B20" s="12" t="s">
         <v>51</v>
       </c>
-      <c r="C20" s="19">
+      <c r="C20" s="12">
         <v>15452.2</v>
       </c>
-      <c r="D20" s="20">
+      <c r="D20" s="13">
         <v>16564.7</v>
       </c>
     </row>
-    <row r="21" spans="1:4" ht="12.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:4" ht="12.95" customHeight="1">
       <c r="A21" s="3" t="s">
         <v>52</v>
       </c>
-      <c r="B21" s="19">
+      <c r="B21" s="12">
         <v>137.5</v>
       </c>
-      <c r="C21" s="19">
+      <c r="C21" s="12">
         <v>135.69999999999999</v>
       </c>
-      <c r="D21" s="20">
+      <c r="D21" s="13">
         <v>132.30000000000001</v>
       </c>
     </row>
-    <row r="22" spans="1:4" ht="23.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:4" ht="23.1" customHeight="1">
       <c r="A22" s="3" t="s">
         <v>53</v>
       </c>
-      <c r="B22" s="19">
+      <c r="B22" s="12">
         <v>30.4</v>
       </c>
-      <c r="C22" s="19">
+      <c r="C22" s="12">
         <v>31.1</v>
       </c>
-      <c r="D22" s="20">
+      <c r="D22" s="13">
         <v>32</v>
       </c>
     </row>
-    <row r="23" spans="1:4" ht="23.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:4" ht="23.1" customHeight="1">
       <c r="A23" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="B23" s="19">
+      <c r="B23" s="12">
         <v>20.2</v>
       </c>
-      <c r="C23" s="19">
+      <c r="C23" s="12">
         <v>20.9</v>
       </c>
-      <c r="D23" s="20">
+      <c r="D23" s="13">
         <v>22.4</v>
       </c>
     </row>
-    <row r="24" spans="1:4" ht="33" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:4" ht="33" customHeight="1">
       <c r="A24" s="3" t="s">
         <v>54</v>
       </c>
-      <c r="B24" s="19">
+      <c r="B24" s="12">
         <v>26.2</v>
       </c>
-      <c r="C24" s="19">
+      <c r="C24" s="12">
         <v>25.9</v>
       </c>
-      <c r="D24" s="20">
+      <c r="D24" s="13">
         <v>25.4</v>
       </c>
     </row>
-    <row r="25" spans="1:4" ht="12.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:4" ht="12.95" customHeight="1">
       <c r="A25" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="B25" s="21"/>
-      <c r="C25" s="21"/>
-      <c r="D25" s="22"/>
-    </row>
-    <row r="26" spans="1:4" ht="12.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B25" s="14"/>
+      <c r="C25" s="14"/>
+      <c r="D25" s="15"/>
+    </row>
+    <row r="26" spans="1:4" ht="12.95" customHeight="1">
       <c r="A26" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="B26" s="21" t="s">
+      <c r="B26" s="14" t="s">
         <v>55</v>
       </c>
-      <c r="C26" s="21" t="s">
+      <c r="C26" s="14" t="s">
         <v>56</v>
       </c>
-      <c r="D26" s="22" t="s">
+      <c r="D26" s="15" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="27" spans="1:4" ht="12.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:4" ht="12.95" customHeight="1">
       <c r="A27" s="6" t="s">
         <v>17</v>
       </c>
-      <c r="B27" s="19">
+      <c r="B27" s="12">
         <v>70</v>
       </c>
-      <c r="C27" s="19">
+      <c r="C27" s="12">
         <v>72.400000000000006</v>
       </c>
-      <c r="D27" s="20">
+      <c r="D27" s="13">
         <v>69.900000000000006</v>
       </c>
     </row>
-    <row r="28" spans="1:4" ht="12.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:4" ht="12.95" customHeight="1">
       <c r="A28" s="3" t="s">
         <v>18</v>
       </c>
@@ -2010,49 +2023,49 @@
       <c r="C28" s="4"/>
       <c r="D28" s="5"/>
     </row>
-    <row r="29" spans="1:4" ht="12.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:4" ht="12.95" customHeight="1">
       <c r="A29" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="B29" s="25" t="s">
+      <c r="B29" s="18" t="s">
         <v>58</v>
       </c>
-      <c r="C29" s="25" t="s">
+      <c r="C29" s="18" t="s">
         <v>59</v>
       </c>
-      <c r="D29" s="26" t="s">
+      <c r="D29" s="19" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="30" spans="1:4" ht="12.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:4" ht="12.95" customHeight="1">
       <c r="A30" s="6" t="s">
         <v>17</v>
       </c>
-      <c r="B30" s="19">
+      <c r="B30" s="12">
         <v>161.4</v>
       </c>
-      <c r="C30" s="19">
+      <c r="C30" s="12">
         <v>162.69999999999999</v>
       </c>
-      <c r="D30" s="20">
+      <c r="D30" s="13">
         <v>158</v>
       </c>
     </row>
-    <row r="31" spans="1:4" ht="12.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:4" ht="12.95" customHeight="1">
       <c r="A31" s="3" t="s">
         <v>61</v>
       </c>
-      <c r="B31" s="25">
+      <c r="B31" s="18">
         <v>19</v>
       </c>
-      <c r="C31" s="25">
+      <c r="C31" s="18">
         <v>18</v>
       </c>
-      <c r="D31" s="26">
+      <c r="D31" s="19">
         <v>22</v>
       </c>
     </row>
-    <row r="32" spans="1:4" ht="12.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:4" ht="12.95" customHeight="1">
       <c r="A32" s="3" t="s">
         <v>62</v>
       </c>
@@ -2060,49 +2073,49 @@
       <c r="C32" s="4"/>
       <c r="D32" s="5"/>
     </row>
-    <row r="33" spans="1:4" ht="12.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:4" ht="12.95" customHeight="1">
       <c r="A33" s="6" t="s">
         <v>19</v>
       </c>
-      <c r="B33" s="19">
+      <c r="B33" s="12">
         <v>5.5</v>
       </c>
-      <c r="C33" s="19">
+      <c r="C33" s="12">
         <v>5.5</v>
       </c>
-      <c r="D33" s="20">
+      <c r="D33" s="13">
         <v>5.3</v>
       </c>
     </row>
-    <row r="34" spans="1:4" ht="12.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:4" ht="12.95" customHeight="1">
       <c r="A34" s="6" t="s">
         <v>17</v>
       </c>
-      <c r="B34" s="19">
+      <c r="B34" s="12">
         <v>131.6</v>
       </c>
-      <c r="C34" s="19">
+      <c r="C34" s="12">
         <v>131.6</v>
       </c>
-      <c r="D34" s="20">
+      <c r="D34" s="13">
         <v>127.7</v>
       </c>
     </row>
-    <row r="35" spans="1:4" ht="12.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:4" ht="12.95" customHeight="1">
       <c r="A35" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="B35" s="25">
+      <c r="B35" s="18">
         <v>67</v>
       </c>
-      <c r="C35" s="25">
+      <c r="C35" s="18">
         <v>69</v>
       </c>
-      <c r="D35" s="26">
+      <c r="D35" s="19">
         <v>65</v>
       </c>
     </row>
-    <row r="36" spans="1:4" ht="12.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:4" ht="12.95" customHeight="1">
       <c r="A36" s="3" t="s">
         <v>63</v>
       </c>
@@ -2110,251 +2123,251 @@
       <c r="C36" s="4"/>
       <c r="D36" s="5"/>
     </row>
-    <row r="37" spans="1:4" ht="12.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:4" ht="12.95" customHeight="1">
       <c r="A37" s="6" t="s">
         <v>19</v>
       </c>
-      <c r="B37" s="19">
+      <c r="B37" s="12">
         <v>14.9</v>
       </c>
-      <c r="C37" s="19">
+      <c r="C37" s="12">
         <v>15.4</v>
       </c>
-      <c r="D37" s="20">
+      <c r="D37" s="13">
         <v>14.8</v>
       </c>
     </row>
-    <row r="38" spans="1:4" ht="12.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:4" ht="12.95" customHeight="1">
       <c r="A38" s="6" t="s">
         <v>17</v>
       </c>
-      <c r="B38" s="19">
+      <c r="B38" s="12">
         <v>354.5</v>
       </c>
-      <c r="C38" s="19">
+      <c r="C38" s="12">
         <v>368.6</v>
       </c>
-      <c r="D38" s="20">
+      <c r="D38" s="13">
         <v>359.1</v>
       </c>
     </row>
-    <row r="39" spans="1:4" ht="12.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:4" ht="12.95" customHeight="1">
       <c r="A39" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="B39" s="25" t="s">
+      <c r="B39" s="18" t="s">
         <v>64</v>
       </c>
-      <c r="C39" s="25" t="s">
+      <c r="C39" s="18" t="s">
         <v>65</v>
       </c>
-      <c r="D39" s="26" t="s">
+      <c r="D39" s="19" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="40" spans="1:4" ht="12.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:4" ht="12.95" customHeight="1">
       <c r="A40" s="7" t="s">
         <v>22</v>
       </c>
-      <c r="B40" s="25"/>
-      <c r="C40" s="25"/>
-      <c r="D40" s="26"/>
-    </row>
-    <row r="41" spans="1:4" ht="12.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B40" s="18"/>
+      <c r="C40" s="18"/>
+      <c r="D40" s="19"/>
+    </row>
+    <row r="41" spans="1:4" ht="12.95" customHeight="1">
       <c r="A41" s="6" t="s">
         <v>23</v>
       </c>
-      <c r="B41" s="25" t="s">
+      <c r="B41" s="18" t="s">
         <v>67</v>
       </c>
-      <c r="C41" s="25" t="s">
+      <c r="C41" s="18" t="s">
         <v>68</v>
       </c>
-      <c r="D41" s="26" t="s">
+      <c r="D41" s="19" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="42" spans="1:4" ht="12.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:4" ht="12.95" customHeight="1">
       <c r="A42" s="6" t="s">
         <v>24</v>
       </c>
-      <c r="B42" s="25" t="s">
+      <c r="B42" s="18" t="s">
         <v>70</v>
       </c>
-      <c r="C42" s="25" t="s">
+      <c r="C42" s="18" t="s">
         <v>71</v>
       </c>
-      <c r="D42" s="26" t="s">
+      <c r="D42" s="19" t="s">
         <v>72</v>
       </c>
     </row>
-    <row r="43" spans="1:4" ht="12.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A43" s="13" t="s">
+    <row r="43" spans="1:4" ht="12.95" customHeight="1">
+      <c r="A43" s="23" t="s">
         <v>73</v>
       </c>
-      <c r="B43" s="14"/>
-      <c r="C43" s="14"/>
-      <c r="D43" s="15"/>
-    </row>
-    <row r="44" spans="1:4" ht="12.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B43" s="24"/>
+      <c r="C43" s="24"/>
+      <c r="D43" s="25"/>
+    </row>
+    <row r="44" spans="1:4" ht="12.95" customHeight="1">
       <c r="A44" s="3" t="s">
         <v>74</v>
       </c>
-      <c r="B44" s="19" t="s">
+      <c r="B44" s="12" t="s">
         <v>75</v>
       </c>
-      <c r="C44" s="19">
+      <c r="C44" s="12">
         <v>20192.599999999999</v>
       </c>
-      <c r="D44" s="20">
+      <c r="D44" s="13">
         <v>18812.7</v>
       </c>
     </row>
-    <row r="45" spans="1:4" ht="23.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:4" ht="23.1" customHeight="1">
       <c r="A45" s="3" t="s">
         <v>76</v>
       </c>
-      <c r="B45" s="19">
+      <c r="B45" s="12">
         <v>32.299999999999997</v>
       </c>
-      <c r="C45" s="19">
+      <c r="C45" s="12">
         <v>40.299999999999997</v>
       </c>
-      <c r="D45" s="20">
+      <c r="D45" s="13">
         <v>39.1</v>
       </c>
     </row>
-    <row r="46" spans="1:4" ht="12.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:4" ht="12.95" customHeight="1">
       <c r="A46" s="7" t="s">
         <v>25</v>
       </c>
-      <c r="B46" s="19"/>
-      <c r="C46" s="19"/>
-      <c r="D46" s="20"/>
-    </row>
-    <row r="47" spans="1:4" ht="12.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B46" s="12"/>
+      <c r="C46" s="12"/>
+      <c r="D46" s="13"/>
+    </row>
+    <row r="47" spans="1:4" ht="12.95" customHeight="1">
       <c r="A47" s="6" t="s">
         <v>26</v>
       </c>
-      <c r="B47" s="19">
+      <c r="B47" s="12">
         <v>14.1</v>
       </c>
-      <c r="C47" s="19">
+      <c r="C47" s="12">
         <v>26.5</v>
       </c>
-      <c r="D47" s="20">
+      <c r="D47" s="13">
         <v>23.4</v>
       </c>
     </row>
-    <row r="48" spans="1:4" ht="12.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:4" ht="12.95" customHeight="1">
       <c r="A48" s="6" t="s">
         <v>27</v>
       </c>
-      <c r="B48" s="19">
+      <c r="B48" s="12">
         <v>14.9</v>
       </c>
-      <c r="C48" s="19">
+      <c r="C48" s="12">
         <v>9.8000000000000007</v>
       </c>
-      <c r="D48" s="20">
+      <c r="D48" s="13">
         <v>11.6</v>
       </c>
     </row>
-    <row r="49" spans="1:4" ht="12.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A49" s="13" t="s">
+    <row r="49" spans="1:4" ht="12.95" customHeight="1">
+      <c r="A49" s="23" t="s">
         <v>28</v>
       </c>
-      <c r="B49" s="14"/>
-      <c r="C49" s="14"/>
-      <c r="D49" s="15"/>
-    </row>
-    <row r="50" spans="1:4" ht="12.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B49" s="24"/>
+      <c r="C49" s="24"/>
+      <c r="D49" s="25"/>
+    </row>
+    <row r="50" spans="1:4" ht="12.95" customHeight="1">
       <c r="A50" s="3" t="s">
         <v>77</v>
       </c>
-      <c r="B50" s="19" t="s">
+      <c r="B50" s="12" t="s">
         <v>78</v>
       </c>
-      <c r="C50" s="19">
+      <c r="C50" s="12">
         <v>393790.9</v>
       </c>
-      <c r="D50" s="20">
+      <c r="D50" s="13">
         <v>420355.7</v>
       </c>
     </row>
-    <row r="51" spans="1:4" ht="12.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:4" ht="12.95" customHeight="1">
       <c r="A51" s="3" t="s">
         <v>79</v>
       </c>
-      <c r="B51" s="19" t="s">
+      <c r="B51" s="12" t="s">
         <v>80</v>
       </c>
-      <c r="C51" s="19">
+      <c r="C51" s="12">
         <v>28933</v>
       </c>
-      <c r="D51" s="20">
+      <c r="D51" s="13">
         <v>23505.599999999999</v>
       </c>
     </row>
-    <row r="52" spans="1:4" ht="12.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:4" ht="12.95" customHeight="1">
       <c r="A52" s="3" t="s">
         <v>81</v>
       </c>
-      <c r="B52" s="19">
+      <c r="B52" s="12">
         <v>53</v>
       </c>
-      <c r="C52" s="19">
+      <c r="C52" s="12">
         <v>53.7</v>
       </c>
-      <c r="D52" s="20">
+      <c r="D52" s="13">
         <v>56.7</v>
       </c>
     </row>
-    <row r="53" spans="1:4" ht="23.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:4" ht="23.1" customHeight="1">
       <c r="A53" s="3" t="s">
         <v>82</v>
       </c>
-      <c r="B53" s="19">
+      <c r="B53" s="12">
         <v>17.8</v>
       </c>
-      <c r="C53" s="19">
+      <c r="C53" s="12">
         <v>19.5</v>
       </c>
-      <c r="D53" s="20">
+      <c r="D53" s="13">
         <v>16.5</v>
       </c>
     </row>
-    <row r="54" spans="1:4" ht="12.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A54" s="13" t="s">
+    <row r="54" spans="1:4" ht="12.95" customHeight="1">
+      <c r="A54" s="23" t="s">
         <v>83</v>
       </c>
-      <c r="B54" s="14"/>
-      <c r="C54" s="14"/>
-      <c r="D54" s="15"/>
-    </row>
-    <row r="55" spans="1:4" ht="23.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B54" s="24"/>
+      <c r="C54" s="24"/>
+      <c r="D54" s="25"/>
+    </row>
+    <row r="55" spans="1:4" ht="23.1" customHeight="1">
       <c r="A55" s="3" t="s">
         <v>84</v>
       </c>
-      <c r="B55" s="25" t="s">
+      <c r="B55" s="18" t="s">
         <v>85</v>
       </c>
-      <c r="C55" s="25" t="s">
+      <c r="C55" s="18" t="s">
         <v>86</v>
       </c>
-      <c r="D55" s="26" t="s">
+      <c r="D55" s="19" t="s">
         <v>87</v>
       </c>
     </row>
-    <row r="56" spans="1:4" ht="12.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A56" s="13" t="s">
+    <row r="56" spans="1:4" ht="12.95" customHeight="1">
+      <c r="A56" s="23" t="s">
         <v>88</v>
       </c>
-      <c r="B56" s="14"/>
-      <c r="C56" s="14"/>
-      <c r="D56" s="15"/>
-    </row>
-    <row r="57" spans="1:4" ht="23.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B56" s="24"/>
+      <c r="C56" s="24"/>
+      <c r="D56" s="25"/>
+    </row>
+    <row r="57" spans="1:4" ht="23.1" customHeight="1">
       <c r="A57" s="3" t="s">
         <v>89</v>
       </c>
@@ -2362,360 +2375,363 @@
       <c r="C57" s="4"/>
       <c r="D57" s="5"/>
     </row>
-    <row r="58" spans="1:4" ht="12.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:4" ht="12.95" customHeight="1">
       <c r="A58" s="6" t="s">
         <v>90</v>
       </c>
-      <c r="B58" s="19" t="s">
+      <c r="B58" s="12" t="s">
         <v>91</v>
       </c>
-      <c r="C58" s="19" t="s">
+      <c r="C58" s="12" t="s">
         <v>91</v>
       </c>
-      <c r="D58" s="20" t="s">
+      <c r="D58" s="13" t="s">
         <v>91</v>
       </c>
     </row>
-    <row r="59" spans="1:4" ht="12.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:4" ht="12.95" customHeight="1">
       <c r="A59" s="6" t="s">
         <v>29</v>
       </c>
-      <c r="B59" s="19" t="s">
+      <c r="B59" s="12" t="s">
         <v>92</v>
       </c>
-      <c r="C59" s="19">
+      <c r="C59" s="12">
         <v>98524.6</v>
       </c>
-      <c r="D59" s="20">
+      <c r="D59" s="13">
         <v>129926.8</v>
       </c>
     </row>
-    <row r="60" spans="1:4" ht="12.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:4" ht="12.95" customHeight="1">
       <c r="A60" s="6" t="s">
         <v>0</v>
       </c>
-      <c r="B60" s="19" t="s">
+      <c r="B60" s="12" t="s">
         <v>93</v>
       </c>
-      <c r="C60" s="19">
+      <c r="C60" s="12">
         <v>12700.2</v>
       </c>
-      <c r="D60" s="20">
+      <c r="D60" s="13">
         <v>13873.7</v>
       </c>
     </row>
-    <row r="61" spans="1:4" ht="23.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:4" ht="23.1" customHeight="1">
       <c r="A61" s="6" t="s">
         <v>94</v>
       </c>
-      <c r="B61" s="19" t="s">
+      <c r="B61" s="12" t="s">
         <v>95</v>
       </c>
-      <c r="C61" s="19">
+      <c r="C61" s="12">
         <v>5107.8</v>
       </c>
-      <c r="D61" s="20">
+      <c r="D61" s="13">
         <v>9090.2000000000007</v>
       </c>
     </row>
-    <row r="62" spans="1:4" ht="12.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A62" s="13" t="s">
+    <row r="62" spans="1:4" ht="12.95" customHeight="1">
+      <c r="A62" s="23" t="s">
         <v>30</v>
       </c>
-      <c r="B62" s="14"/>
-      <c r="C62" s="14"/>
-      <c r="D62" s="15"/>
-    </row>
-    <row r="63" spans="1:4" ht="23.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B62" s="24"/>
+      <c r="C62" s="24"/>
+      <c r="D62" s="25"/>
+    </row>
+    <row r="63" spans="1:4" ht="23.1" customHeight="1">
       <c r="A63" s="3" t="s">
         <v>96</v>
       </c>
-      <c r="B63" s="19" t="s">
+      <c r="B63" s="12" t="s">
         <v>97</v>
       </c>
-      <c r="C63" s="19">
+      <c r="C63" s="12">
         <v>3354.4</v>
       </c>
-      <c r="D63" s="20">
+      <c r="D63" s="13">
         <v>3496.1</v>
       </c>
     </row>
-    <row r="64" spans="1:4" ht="12.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:4" ht="12.95" customHeight="1">
       <c r="A64" s="3" t="s">
         <v>98</v>
       </c>
-      <c r="B64" s="19">
+      <c r="B64" s="12">
         <v>216.3</v>
       </c>
-      <c r="C64" s="19">
+      <c r="C64" s="12">
         <v>187.2</v>
       </c>
-      <c r="D64" s="20">
+      <c r="D64" s="13">
         <v>241.9</v>
       </c>
     </row>
-    <row r="65" spans="1:4" ht="12.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:4" ht="12.95" customHeight="1">
       <c r="A65" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="B65" s="25" t="s">
+      <c r="B65" s="18" t="s">
         <v>99</v>
       </c>
-      <c r="C65" s="25">
+      <c r="C65" s="18">
         <v>3109</v>
       </c>
-      <c r="D65" s="26" t="s">
+      <c r="D65" s="19" t="s">
         <v>100</v>
       </c>
     </row>
-    <row r="66" spans="1:4" ht="12.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:4" ht="12.95" customHeight="1">
       <c r="A66" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="B66" s="25"/>
-      <c r="C66" s="25"/>
-      <c r="D66" s="26"/>
-    </row>
-    <row r="67" spans="1:4" ht="12.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B66" s="18"/>
+      <c r="C66" s="18"/>
+      <c r="D66" s="19"/>
+    </row>
+    <row r="67" spans="1:4" ht="12.95" customHeight="1">
       <c r="A67" s="6" t="s">
         <v>101</v>
       </c>
-      <c r="B67" s="25">
+      <c r="B67" s="18">
         <v>730</v>
       </c>
-      <c r="C67" s="25">
+      <c r="C67" s="18">
         <v>695</v>
       </c>
-      <c r="D67" s="26">
+      <c r="D67" s="19">
         <v>540</v>
       </c>
     </row>
-    <row r="68" spans="1:4" ht="12.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:4" ht="12.95" customHeight="1">
       <c r="A68" s="6" t="s">
         <v>102</v>
       </c>
-      <c r="B68" s="25" t="s">
+      <c r="B68" s="18" t="s">
         <v>33</v>
       </c>
-      <c r="C68" s="25" t="s">
+      <c r="C68" s="18" t="s">
         <v>103</v>
       </c>
-      <c r="D68" s="26">
+      <c r="D68" s="19">
         <v>102</v>
       </c>
     </row>
-    <row r="69" spans="1:4" ht="12.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:4" ht="12.95" customHeight="1">
       <c r="A69" s="6" t="s">
         <v>34</v>
       </c>
-      <c r="B69" s="25" t="s">
+      <c r="B69" s="18" t="s">
         <v>33</v>
       </c>
-      <c r="C69" s="25" t="s">
+      <c r="C69" s="18" t="s">
         <v>33</v>
       </c>
-      <c r="D69" s="26" t="s">
+      <c r="D69" s="19" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="70" spans="1:4" ht="12.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:4" ht="12.95" customHeight="1">
       <c r="A70" s="6" t="s">
         <v>104</v>
       </c>
-      <c r="B70" s="25">
+      <c r="B70" s="18">
         <v>270</v>
       </c>
-      <c r="C70" s="25" t="s">
+      <c r="C70" s="18" t="s">
         <v>33</v>
       </c>
-      <c r="D70" s="26" t="s">
+      <c r="D70" s="19" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="71" spans="1:4" ht="12.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:4" ht="12.95" customHeight="1">
       <c r="A71" s="6" t="s">
         <v>105</v>
       </c>
-      <c r="B71" s="25" t="s">
+      <c r="B71" s="18" t="s">
         <v>33</v>
       </c>
-      <c r="C71" s="25" t="s">
+      <c r="C71" s="18" t="s">
         <v>33</v>
       </c>
-      <c r="D71" s="26" t="s">
+      <c r="D71" s="19" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="72" spans="1:4" ht="12.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:4" ht="12.95" customHeight="1">
       <c r="A72" s="6" t="s">
         <v>106</v>
       </c>
-      <c r="B72" s="19">
+      <c r="B72" s="12">
         <v>3</v>
       </c>
-      <c r="C72" s="19">
+      <c r="C72" s="12">
         <v>5</v>
       </c>
-      <c r="D72" s="20">
+      <c r="D72" s="13">
         <v>7.4</v>
       </c>
     </row>
-    <row r="73" spans="1:4" ht="12.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:4" ht="12.95" customHeight="1">
       <c r="A73" s="6" t="s">
         <v>35</v>
       </c>
-      <c r="B73" s="25">
+      <c r="B73" s="18">
         <v>49</v>
       </c>
-      <c r="C73" s="25" t="s">
+      <c r="C73" s="18" t="s">
         <v>33</v>
       </c>
-      <c r="D73" s="26" t="s">
+      <c r="D73" s="19" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="74" spans="1:4" ht="12.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:4" ht="12.95" customHeight="1">
       <c r="A74" s="6" t="s">
         <v>107</v>
       </c>
-      <c r="B74" s="25">
+      <c r="B74" s="18">
         <v>1</v>
       </c>
-      <c r="C74" s="25" t="s">
+      <c r="C74" s="18" t="s">
         <v>33</v>
       </c>
-      <c r="D74" s="26" t="s">
+      <c r="D74" s="19" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="75" spans="1:4" ht="12.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:4" ht="12.95" customHeight="1">
       <c r="A75" s="6" t="s">
         <v>108</v>
       </c>
-      <c r="B75" s="25" t="s">
+      <c r="B75" s="18" t="s">
         <v>33</v>
       </c>
-      <c r="C75" s="25" t="s">
+      <c r="C75" s="18" t="s">
         <v>33</v>
       </c>
-      <c r="D75" s="26" t="s">
+      <c r="D75" s="19" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="76" spans="1:4" ht="12.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A76" s="13" t="s">
+    <row r="76" spans="1:4" ht="12.95" customHeight="1">
+      <c r="A76" s="23" t="s">
         <v>109</v>
       </c>
-      <c r="B76" s="14"/>
-      <c r="C76" s="14"/>
-      <c r="D76" s="15"/>
-    </row>
-    <row r="77" spans="1:4" ht="23.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B76" s="24"/>
+      <c r="C76" s="24"/>
+      <c r="D76" s="25"/>
+    </row>
+    <row r="77" spans="1:4" ht="23.1" customHeight="1">
       <c r="A77" s="3" t="s">
         <v>110</v>
       </c>
-      <c r="B77" s="19" t="s">
+      <c r="B77" s="12" t="s">
         <v>111</v>
       </c>
-      <c r="C77" s="19">
+      <c r="C77" s="12">
         <v>53833.5</v>
       </c>
-      <c r="D77" s="20">
+      <c r="D77" s="13">
         <v>67878.399999999994</v>
       </c>
     </row>
-    <row r="78" spans="1:4" ht="23.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:4" ht="23.1" customHeight="1">
       <c r="A78" s="3" t="s">
         <v>36</v>
       </c>
-      <c r="B78" s="19">
+      <c r="B78" s="12">
         <v>100</v>
       </c>
-      <c r="C78" s="19">
+      <c r="C78" s="12">
         <v>107.3</v>
       </c>
-      <c r="D78" s="20">
+      <c r="D78" s="13">
         <v>116.6</v>
       </c>
     </row>
-    <row r="79" spans="1:4" ht="12.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:4" ht="12.95" customHeight="1">
       <c r="A79" s="3" t="s">
         <v>112</v>
       </c>
-      <c r="B79" s="19" t="s">
+      <c r="B79" s="12" t="s">
         <v>113</v>
       </c>
-      <c r="C79" s="19">
+      <c r="C79" s="12">
         <v>961</v>
       </c>
-      <c r="D79" s="20">
+      <c r="D79" s="13">
         <v>1257.2</v>
       </c>
     </row>
-    <row r="80" spans="1:4" ht="23.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:4" ht="23.1" customHeight="1">
       <c r="A80" s="8" t="s">
         <v>37</v>
       </c>
-      <c r="B80" s="23">
+      <c r="B80" s="16">
         <v>117.9</v>
       </c>
-      <c r="C80" s="23">
+      <c r="C80" s="16">
         <v>90.5</v>
       </c>
-      <c r="D80" s="24">
+      <c r="D80" s="17">
         <v>126.5</v>
       </c>
     </row>
-    <row r="81" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A81" s="27" t="s">
+    <row r="81" spans="1:4">
+      <c r="A81" s="26" t="s">
         <v>114</v>
       </c>
-      <c r="B81" s="27"/>
-      <c r="C81" s="27"/>
-      <c r="D81" s="27"/>
-    </row>
-    <row r="82" spans="1:4" ht="12" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A82" s="28" t="s">
+      <c r="B81" s="26"/>
+      <c r="C81" s="26"/>
+      <c r="D81" s="26"/>
+    </row>
+    <row r="82" spans="1:4" ht="12" customHeight="1">
+      <c r="A82" s="21" t="s">
         <v>115</v>
       </c>
-      <c r="B82" s="28"/>
-      <c r="C82" s="28"/>
-      <c r="D82" s="28"/>
-    </row>
-    <row r="83" spans="1:4" ht="12" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A83" s="28" t="s">
+      <c r="B82" s="21"/>
+      <c r="C82" s="21"/>
+      <c r="D82" s="21"/>
+    </row>
+    <row r="83" spans="1:4" ht="12" customHeight="1">
+      <c r="A83" s="21" t="s">
         <v>116</v>
       </c>
-      <c r="B83" s="28"/>
-      <c r="C83" s="28"/>
-      <c r="D83" s="28"/>
-    </row>
-    <row r="84" spans="1:4" ht="12" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A84" s="28" t="s">
+      <c r="B83" s="21"/>
+      <c r="C83" s="21"/>
+      <c r="D83" s="21"/>
+    </row>
+    <row r="84" spans="1:4" ht="12" customHeight="1">
+      <c r="A84" s="21" t="s">
         <v>117</v>
       </c>
-      <c r="B84" s="28"/>
-      <c r="C84" s="28"/>
-      <c r="D84" s="28"/>
-    </row>
-    <row r="85" spans="1:4" ht="12" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A85" s="28" t="s">
+      <c r="B84" s="21"/>
+      <c r="C84" s="21"/>
+      <c r="D84" s="21"/>
+    </row>
+    <row r="85" spans="1:4" ht="12" customHeight="1">
+      <c r="A85" s="21" t="s">
         <v>118</v>
       </c>
-      <c r="B85" s="28"/>
-      <c r="C85" s="28"/>
-      <c r="D85" s="28"/>
-    </row>
-    <row r="86" spans="1:4" s="30" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A86" s="29" t="s">
+      <c r="B85" s="21"/>
+      <c r="C85" s="21"/>
+      <c r="D85" s="21"/>
+    </row>
+    <row r="86" spans="1:4" s="20" customFormat="1" ht="20.100000000000001" customHeight="1">
+      <c r="A86" s="22" t="s">
         <v>119</v>
       </c>
-      <c r="B86" s="29"/>
-      <c r="C86" s="29"/>
-      <c r="D86" s="29"/>
+      <c r="B86" s="22"/>
+      <c r="C86" s="22"/>
+      <c r="D86" s="22"/>
     </row>
   </sheetData>
   <mergeCells count="16">
+    <mergeCell ref="A1:D1"/>
+    <mergeCell ref="A3:D3"/>
+    <mergeCell ref="A14:D14"/>
     <mergeCell ref="A85:D85"/>
     <mergeCell ref="A86:D86"/>
     <mergeCell ref="A18:D18"/>
@@ -2729,9 +2745,6 @@
     <mergeCell ref="A82:D82"/>
     <mergeCell ref="A83:D83"/>
     <mergeCell ref="A84:D84"/>
-    <mergeCell ref="A1:D1"/>
-    <mergeCell ref="A3:D3"/>
-    <mergeCell ref="A14:D14"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>